<commit_message>
Attempted using pandas to present the data - still can't figure out how to work with jpg.
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -28,199 +28,190 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Acoustic Guitar.  Black edition! Brand new in box/plastic packaging. Concert sizes. 38inch - $55 41inch - $65 (Sold) Without guitar case.  Add-on accessories available: 1 string : $2 Set of 6 strings: $6 (Metal) Capo : $6 Set of plastic picks with holder: $1 Music stand: $12 Conductor stand: $20  bu</t>
-  </si>
-  <si>
-    <t>S$55</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/acoustic-black-guitar-1052300278/</t>
-  </si>
-  <si>
-    <t>very seasonal tone. solid top. made in 70s. come with bag.</t>
-  </si>
-  <si>
-    <t>S$215</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/70s-japan-made-classical-guitar-1052294194/</t>
-  </si>
-  <si>
-    <t>Working Condition: 10/10 Physical Condition: 9/10 ⬇️ This is a very versatile and one of the best electric guitar I played. It looks very good with the upgraded original Suhr black hardware. Definitely worth the money! Comes with the original Suhr padded gig bag and the spec sheet.  Open for trade w</t>
-  </si>
-  <si>
-    <t>S$3,400</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/usa-suhr-modern-satin-electric-guitar-1052293193/</t>
-  </si>
-  <si>
-    <t>Features Series: Squier Artist Series Body: Basswood Neck: Maple, C-Shape, Satin Polyurethane Finish Fingerboard: Rosewood, 9.5" Radius (241 mm) No. of Frets: 22 Medium Jumbo Pickups: 1 Dual-Coil Humbucking Pickup Controls: Volume Pickup Switching: 3-Position Blade: Position 1. Front Coil Position 2</t>
+    <t>Cort Acoustic Guitar Missing E string In good condition  **Fast deal within 24 Hour at $50**</t>
+  </si>
+  <si>
+    <t>S$70</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/acoustic-guitar-1052519327/</t>
+  </si>
+  <si>
+    <t>Bought for $300+ letting it go for $140 still in very good condition comes with guitar bag+tuner.Fast deal $130</t>
+  </si>
+  <si>
+    <t>S$140</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/manning-guitar-1045632026/</t>
+  </si>
+  <si>
+    <t>Excellent condition. Used only for self hobby and is grossly under-utilized. Selling as I am moving back to acoustic playing. Hope this fabulous item will soon find a new owner to enjoy this amazing Effect Processor. Complete with User Instructions.</t>
+  </si>
+  <si>
+    <t>S$400</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/boss-gt-6-guitar-effect-processor-1037688896/</t>
+  </si>
+  <si>
+    <t>still in great condition but the pick up switch slightly lose. comes with the guitar bag. can slightly nego!</t>
+  </si>
+  <si>
+    <t>S$150</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/yamaha-electric-guitar-1052496434/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With guitar bag </t>
+  </si>
+  <si>
+    <t>S$390</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/yamaha-guitar-1052492764/</t>
+  </si>
+  <si>
+    <t>As new condition</t>
+  </si>
+  <si>
+    <t>S$250</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/jasmine-by-takamine-c23-classical-guitar-1052492556/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Good condition  Only played a few times Strings are half metal half plastic Suitable for starter Self collect Thank you </t>
+  </si>
+  <si>
+    <t>S$80</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/just-another-lovely-guitar-🎸-80-free-leather-case-1051449182/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightly used.  Didn’t use it for a long time.  Good for beginners. No bag, cash and carry.  </t>
+  </si>
+  <si>
+    <t>carousell.sg/p/zen-guitar-1052485831/</t>
+  </si>
+  <si>
+    <t>🎸Pm me how much you are willing to buy it for 🎸Literally BN and have never brought it out for any events or leisure playing. 🎸Condition: 10/10, no scratches and strings has been changed recently and they are from Yamaha 🎸just didn’t like the guitar after buying it and hope someone who is more suitab</t>
+  </si>
+  <si>
+    <t>S$0</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/greg-bennett-semi-acoustic-guitar-1052482212/</t>
+  </si>
+  <si>
+    <t>Light use,  Price is negotiable.  If interested, please PM me</t>
+  </si>
+  <si>
+    <t>S$399</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/yamaha-fg700s-guitar-1052478052/</t>
+  </si>
+  <si>
+    <t>Lightly used. It was purchased in March 2020 at the original price of $159. Comes together with the bag. Meet up at Aljunied MRT</t>
+  </si>
+  <si>
+    <t>S$100</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/yamaha-c40-classical-guitar-1052474643/</t>
+  </si>
+  <si>
+    <t>Brand New Acoustics 6 steel string Beginner Guitar 38 inches   Orginal Price $85 Now $65 only come with bag (for 1pc only)   Guitar +bag =$65  This guitar is best for beginners with features : -low fret action for ease of pressing  -soft string, not hard to press  -portable, 38 inches in size not to</t>
+  </si>
+  <si>
+    <t>S$65</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/brand-new-38-inch-beginner-acoustic-guitar-cut-away-1012184300/</t>
+  </si>
+  <si>
+    <t>missing whammy  bar. New pack of string will be provided.  no bag  only guitar</t>
+  </si>
+  <si>
+    <t>S$120</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/rockstar-guitar-1052460141/</t>
+  </si>
+  <si>
+    <t>I-Suzuki classical guitar signed by fjngerstlye guitarist Akihiro Tanaka. No damage, full working condition. Selling to make space at home.</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/classical-guitar-signed-by-akihiro-tanaka-1052451722/</t>
+  </si>
+  <si>
+    <t>Mint condition,contact 96994466</t>
+  </si>
+  <si>
+    <t>S$2,300</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/gibson-montana-2020-j-15-acoustic-guitar-walnut-natural-1052450145/</t>
+  </si>
+  <si>
+    <t>used for about a year fasr deal at $100 negotiatable</t>
+  </si>
+  <si>
+    <t>S$110</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/acoustic-guitar-1052434160/</t>
+  </si>
+  <si>
+    <t>Ibanez Electric Guitar 🎸 RG321MH made in Korea. The body is made of solid mahogany. It has beautiful Rosewood fingerboard with pearl inlay dots. The neck is 3 piece maple Wizard II neck with rare 430mm/17inch radius neck, which is flattest type of neck in Ibanez line only found in Prestige models th</t>
   </si>
   <si>
     <t>S$350</t>
   </si>
   <si>
-    <t>carousell.sg/p/fender-squier-avril-lavigne-telecaster-electric-guitar-1052287784/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Just laying around the house. Selling it off as it’s collecting dust and space. Works great. Strings fine. Very beautiful piece. Non negotiable price. </t>
-  </si>
-  <si>
-    <t>S$130</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/acoustic-guitar-1052284610/</t>
-  </si>
-  <si>
-    <t>Sitka spruce and rosewood guitar acoustic  with plug in.</t>
-  </si>
-  <si>
-    <t>S$185</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/guitar-acoustic-1052269711/</t>
-  </si>
-  <si>
-    <t>🌟Good condition.  ✨Selling as a bundle✨ 🐺 Monster High Clawdeen wolf costume 🧊 Monster High Abbey Bominable costume 🌟Sold🌟🎸 Monster High blue guitar  🚘 Monster High purple car 📷Monster High bracelet + doll brush + photo frame with picture inside 👝 Monster High pouch 🧩 Monster High puzzle  Monster Hi</t>
-  </si>
-  <si>
-    <t>S$37S$40</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/monster-high-clearance-costumes-guitar-toy-car-1039129080/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Self collect </t>
-  </si>
-  <si>
-    <t>S$120</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/artists-brand-new-guitar-for-sale-1052262200/</t>
-  </si>
-  <si>
-    <t>Maestro Standard Series [SD-1] Top: Laminated Spruce  Sides: Mahogany  Back: Mahogany Neck: Nato   Pre-loved Maestro guitar. Good condition. Selling to make space in my room and looking for someone to put it into good use (: Meet-up only. I’ll go to you ^^</t>
-  </si>
-  <si>
-    <t>S$80</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/pre-loved-maestro-sd-1-guitar-1052260541/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solid wood mahogany. Spruce top  Old elixir strings need changing Major crack at the base as it was dropped </t>
-  </si>
-  <si>
-    <t>S$199</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/segovia-acoustic-guitar-1052257541/</t>
-  </si>
-  <si>
-    <t>Natural wood colour  Full size Brand new in box  Walk-in purchase Edventure Music School Pte Ltd (Tampines) 433, #01-67 Tampines Street 43, 520433 9889 0433 https://goo.gl/maps/4hGCLc7H9kaPPnwKA</t>
-  </si>
-  <si>
-    <t>S$90</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/classical-guitar-full-size-1052254932/</t>
-  </si>
-  <si>
-    <t>Bought this kid-sized guitar hoping to arouse my children's interest in music. As they have more sports genes and also have out grown, so, we are letting it go.  Brand : Lark, Shanghai, China Artice no : UC202 Content : 4-string guitar which comes with a red plectrum Total length  : 23 inches  Scale</t>
-  </si>
-  <si>
-    <t>S$15</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/lark-uc202-4-string-guitar-23-inches-for-kids-1052251264/</t>
-  </si>
-  <si>
-    <t>Condition 9/10 Korean Brand. One chip at the bottom as seen in the last picture. Last string in first picture is missing but actual guitar has all 6 strings.  Strings on guitar is Elixir strings and are used. Recently polished guitar and fretboard. Good for beginners Comes with guitar Bag and one pi</t>
-  </si>
-  <si>
-    <t>S$100</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/swing-rose-65-acoustic-guitar-1052248777/</t>
-  </si>
-  <si>
-    <t>pm for more info</t>
-  </si>
-  <si>
-    <t>S$75</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/babilon-guitar-1052237462/</t>
-  </si>
-  <si>
-    <t>Jack and Danny Brothers Model No: C-36  1/2 used but in good condition no scratches or dents open for negotiations with a quick deal 😁</t>
-  </si>
-  <si>
-    <t>S$70</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/classical-guitar-1043044552/</t>
-  </si>
-  <si>
-    <t>🔥Product is in stock 🔥 Shipment done within 2 days  ⚜Ukulele special designed coloured guitars, Enjoy crystal-clear sound.  ⚜Lightweight and excellent to the touch.  ⚜Easy to carry and can be used for a long time.  ⚜It is an addicting instrument that can be taken everywhere.  ⚜Best choice for you, o</t>
-  </si>
-  <si>
-    <t>S$28</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/sg-instocks-23-inch-hawaiian-guitar-soprano-ukulele-4-strings-uke-string-pick-for-beginners-kid-gift-1052230882/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totally still in good and new condition, let go because seldom use.  free bag, capo and guitar pick. </t>
-  </si>
-  <si>
-    <t>carousell.sg/p/acoustic-guitar-1052229051/</t>
-  </si>
-  <si>
-    <t>-Gibson 2016 Les Paul Studio HP Electric Guitar w/Case, Wine Red -Will need to replace string -Rarely used -No lowballing pls -Self-pickup</t>
-  </si>
-  <si>
-    <t>S$2,500</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/gibson-2016-les-paul-studio-hp-electric-guitar-w-case-wine-red-1052225491/</t>
-  </si>
-  <si>
-    <t>Item is completely brand new. (Not tested)  Seller will not be responsible for any issue pertaining to this equipment.  Collection only at 821174 blk A COD</t>
-  </si>
-  <si>
-    <t>S$12</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/electric-guitar-double-coil-pickup-humbucker-1052219048/</t>
-  </si>
-  <si>
-    <t>Selling Epiphone semi acoustic guitar Pro-1 Ultra. Condition 9.5/10. Built-in pickup and electronics working well. Comes with guitar bag and capo.</t>
-  </si>
-  <si>
-    <t>S$260</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/epiphone-electro-acoustic-guitar-1052217961/</t>
-  </si>
-  <si>
-    <t>this is a custom made gretsch baritone, it has a small chip at the back but it works perfectly fine. selling it off because I bought a new guitar and i hope to find a new home for this baby. Got this at $950 and the price is negotiable from $600 plus it will come with a hardcase.</t>
-  </si>
-  <si>
-    <t>S$600</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/electric-guitar-1052215027/</t>
-  </si>
-  <si>
-    <t>Brand New Acoustics 6 steel string Beginner Guitar 38 inches   Orginal Price $85 Now $65 only come with bag (for 1pc only)   Guitar +bag =$65  This guitar is best for beginners with features : -low fret action for ease of pressing  -soft string, not hard to press  -portable, 38 inches in size not to</t>
-  </si>
-  <si>
-    <t>S$65</t>
-  </si>
-  <si>
-    <t>carousell.sg/p/brand-new-38-inch-beginner-acoustic-guitar-cut-away-1012184300/</t>
+    <t>carousell.sg/p/ibanez-electric-guitar-rg321mh-made-in-korea-1052433450/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almost brand new vemuram jan ray effects pedal. Bought from davis guitar on 12 Nov. Letting it go as it doesnt really fit my needs. Brand new price is $495  It is used to simulate the sound of a fender blackface amp and it does that job spectacularly. Don’t really need it as i already have a fender </t>
+  </si>
+  <si>
+    <t>S$420</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/vemuram-jan-ray-guitar-effects-pedal-1052433145/</t>
+  </si>
+  <si>
+    <t>Guitar bag will be provided too!</t>
+  </si>
+  <si>
+    <t>S$50</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/beginner-guitar-pink-1052430606/</t>
+  </si>
+  <si>
+    <t>almost new condition.  solid Engelmann spruce top solid mahogany back and sides abalone rosette neck and body binding 42.5mm saddle width 645mm scale length cutaway design Fishman Sonicore pickup with Ibanez SST preamp integrated tuner chrome grover tuning machines Colour: Natural</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/ibanez-full-solid-acoustic-electric-guitar-1052428858/</t>
+  </si>
+  <si>
+    <t>Still in great condition. 4 stringed bass guitar. Can test before purchase. Collect from my place 3 min from admiralty mrt station</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/electric-tgm-bass-guitar-with-case-and-strap-1052407955/</t>
+  </si>
+  <si>
+    <t>Will fit all Fender guitars.  Stratocaster telecaster jaguar jazzmaster.  Priced cheap to clear space. I want to be able to use my house.</t>
+  </si>
+  <si>
+    <t>S$67</t>
+  </si>
+  <si>
+    <t>carousell.sg/p/hardcase-for-fender-guitars-1052399345/</t>
   </si>
 </sst>
 </file>
@@ -654,164 +645,164 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>